<commit_message>
Update analyses and figures with latest changes
</commit_message>
<xml_diff>
--- a/outputs/excel/abe_replication.xlsx
+++ b/outputs/excel/abe_replication.xlsx
@@ -458,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,6 +562,44 @@
       </c>
       <c r="E5" t="n">
         <v>506.97</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>39.37802291047942</v>
+      </c>
+      <c r="C6" t="n">
+        <v>13.41103145474985</v>
+      </c>
+      <c r="D6" t="n">
+        <v>17</v>
+      </c>
+      <c r="E6" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Gender (0: F | 1: M)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5803988120492151</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.4935984192187962</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +659,7 @@
         <v>0.57</v>
       </c>
       <c r="D3" t="n">
-        <v>0.57</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -637,7 +675,7 @@
         <v>0.99</v>
       </c>
       <c r="D4" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="6">
@@ -653,7 +691,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>2.98</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="7">
@@ -669,7 +707,7 @@
         <v>0.71</v>
       </c>
       <c r="D7" t="n">
-        <v>0.73</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="9">
@@ -745,7 +783,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -764,7 +802,7 @@
       <c r="D1" s="3" t="n"/>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>HB M2 (with a covariate)</t>
+          <t>HB M2 (with 3 covariates)</t>
         </is>
       </c>
       <c r="F1" s="2" t="n"/>
@@ -819,183 +857,247 @@
         <v>-3.34</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.76</v>
+        <v>-3.86</v>
       </c>
       <c r="F4" t="n">
-        <v>-3.59</v>
+        <v>-3.64</v>
       </c>
       <c r="G4" t="n">
-        <v>-3.41</v>
+        <v>-3.44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Purchase rate log(λ) - Initial amount ($ 10^-3)</t>
+          <t>Purchase rate log(λ) - first.sales</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Dropout rate log(μ) - Intercept</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>-4.21</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-3.7</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-3.31</v>
+          <t>Purchase rate log(λ) - age scaled</t>
+        </is>
       </c>
       <c r="E6" t="n">
-        <v>-3.99</v>
+        <v>-0.26</v>
       </c>
       <c r="F6" t="n">
-        <v>-3.62</v>
+        <v>-0.11</v>
       </c>
       <c r="G6" t="n">
-        <v>-3.38</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Dropout rate log(μ) - Initial amount ($ 10^-3)</t>
+          <t>Purchase rate log(λ) - gender binary</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-0.22</v>
+        <v>-0.12</v>
       </c>
       <c r="F7" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="G7" t="n">
-        <v>0.21</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>sigma^2_λ = var[log λ]</t>
+          <t>Dropout rate log(μ) - Intercept</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.1</v>
+        <v>-4.21</v>
       </c>
       <c r="C8" t="n">
-        <v>1.37</v>
+        <v>-3.7</v>
       </c>
       <c r="D8" t="n">
-        <v>1.74</v>
+        <v>-3.31</v>
       </c>
       <c r="E8" t="n">
-        <v>1.11</v>
+        <v>-4.61</v>
       </c>
       <c r="F8" t="n">
-        <v>1.36</v>
+        <v>-3.96</v>
       </c>
       <c r="G8" t="n">
-        <v>1.64</v>
+        <v>-3.53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>sigma^2_μ = var[log μ]</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.14</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.01</v>
+          <t>Dropout rate log(μ) - first.sales</t>
+        </is>
       </c>
       <c r="E9" t="n">
-        <v>-0.19</v>
+        <v>-0.35</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="G9" t="n">
-        <v>0.49</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>sigma_λ_μ = cov[log λ, log μ]</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>2.23</v>
-      </c>
-      <c r="C10" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D10" t="n">
-        <v>6.08</v>
+          <t>Dropout rate log(μ) - age scaled</t>
+        </is>
       </c>
       <c r="E10" t="n">
-        <v>0.9399999999999999</v>
+        <v>-0.16</v>
       </c>
       <c r="F10" t="n">
-        <v>1.82</v>
+        <v>0.1</v>
       </c>
       <c r="G10" t="n">
-        <v>3.83</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Correlation computed from Γ₀</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>-0.07000000000000001</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.36</v>
+          <t>Dropout rate log(μ) - gender binary</t>
+        </is>
       </c>
       <c r="E11" t="n">
-        <v>-0.13</v>
+        <v>-0.14</v>
       </c>
       <c r="F11" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="G11" t="n">
-        <v>0.26</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
+          <t>sigma^2_λ = var[log λ]</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>sigma^2_μ = var[log μ]</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.21</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>sigma_λ_μ = cov[log λ, log μ]</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6.08</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Correlation computed from Γ₀</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.14</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
           <t>Marginal log-likelihood</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C16" t="n">
         <v>-14955</v>
       </c>
-      <c r="F12" t="n">
-        <v>-14954</v>
+      <c r="F16" t="n">
+        <v>-15070</v>
       </c>
     </row>
   </sheetData>
@@ -1083,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.754</v>
+        <v>0.753</v>
       </c>
       <c r="C2" t="n">
         <v>0.487</v>
@@ -1092,25 +1194,25 @@
         <v>1.085</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0161</v>
+        <v>0.0163</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0007</v>
+        <v>0.0009</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0717</v>
+        <v>0.0683</v>
       </c>
       <c r="H2" t="n">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="I2" t="n">
-        <v>0.433</v>
+        <v>0.429</v>
       </c>
       <c r="J2" t="n">
         <v>0.998</v>
       </c>
       <c r="K2" t="n">
-        <v>21.78</v>
+        <v>21.69</v>
       </c>
     </row>
     <row r="3">
@@ -1121,31 +1223,31 @@
         <v>0.698</v>
       </c>
       <c r="C3" t="n">
-        <v>0.465</v>
+        <v>0.459</v>
       </c>
       <c r="D3" t="n">
-        <v>0.987</v>
+        <v>0.988</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0145</v>
+        <v>0.0166</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0007</v>
+        <v>0.0011</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0602</v>
+        <v>0.065</v>
       </c>
       <c r="H3" t="n">
-        <v>1.33</v>
+        <v>1.16</v>
       </c>
       <c r="I3" t="n">
-        <v>0.471</v>
+        <v>0.421</v>
       </c>
       <c r="J3" t="n">
-        <v>0.995</v>
+        <v>0.996</v>
       </c>
       <c r="K3" t="n">
-        <v>20.7</v>
+        <v>19.93</v>
       </c>
     </row>
     <row r="4">
@@ -1153,34 +1255,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.513</v>
+        <v>0.498</v>
       </c>
       <c r="C4" t="n">
-        <v>0.29</v>
+        <v>0.292</v>
       </c>
       <c r="D4" t="n">
-        <v>0.793</v>
+        <v>0.758</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0164</v>
+        <v>0.0136</v>
       </c>
       <c r="F4" t="n">
         <v>0.0007</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07190000000000001</v>
+        <v>0.0574</v>
       </c>
       <c r="H4" t="n">
-        <v>1.17</v>
+        <v>1.42</v>
       </c>
       <c r="I4" t="n">
-        <v>0.425</v>
+        <v>0.494</v>
       </c>
       <c r="J4" t="n">
-        <v>0.992</v>
+        <v>0.998</v>
       </c>
       <c r="K4" t="n">
-        <v>14.66</v>
+        <v>15.05</v>
       </c>
     </row>
     <row r="5">
@@ -1188,34 +1290,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.493</v>
+        <v>0.515</v>
       </c>
       <c r="C5" t="n">
-        <v>0.293</v>
+        <v>0.291</v>
       </c>
       <c r="D5" t="n">
-        <v>0.75</v>
+        <v>0.798</v>
       </c>
       <c r="E5" t="n">
-        <v>0.015</v>
+        <v>0.0152</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.0008</v>
       </c>
       <c r="G5" t="n">
-        <v>0.06270000000000001</v>
+        <v>0.0645</v>
       </c>
       <c r="H5" t="n">
-        <v>1.29</v>
+        <v>1.26</v>
       </c>
       <c r="I5" t="n">
-        <v>0.459</v>
+        <v>0.453</v>
       </c>
       <c r="J5" t="n">
-        <v>0.998</v>
+        <v>0.992</v>
       </c>
       <c r="K5" t="n">
-        <v>14.54</v>
+        <v>15.03</v>
       </c>
     </row>
     <row r="6">
@@ -1223,34 +1325,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.446</v>
+        <v>0.448</v>
       </c>
       <c r="C6" t="n">
-        <v>0.259</v>
+        <v>0.26</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0148</v>
+        <v>0.0138</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.0007</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0644</v>
+        <v>0.0568</v>
       </c>
       <c r="H6" t="n">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="I6" t="n">
-        <v>0.462</v>
+        <v>0.489</v>
       </c>
       <c r="J6" t="n">
-        <v>0.987</v>
+        <v>0.988</v>
       </c>
       <c r="K6" t="n">
-        <v>13.04</v>
+        <v>13.36</v>
       </c>
     </row>
     <row r="7">
@@ -1258,34 +1360,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.389</v>
+        <v>0.394</v>
       </c>
       <c r="C7" t="n">
-        <v>0.206</v>
+        <v>0.209</v>
       </c>
       <c r="D7" t="n">
-        <v>0.63</v>
+        <v>0.638</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0159</v>
+        <v>0.0146</v>
       </c>
       <c r="F7" t="n">
         <v>0.0007</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0712</v>
+        <v>0.0634</v>
       </c>
       <c r="H7" t="n">
-        <v>1.21</v>
+        <v>1.31</v>
       </c>
       <c r="I7" t="n">
-        <v>0.437</v>
+        <v>0.467</v>
       </c>
       <c r="J7" t="n">
-        <v>0.981</v>
+        <v>0.983</v>
       </c>
       <c r="K7" t="n">
-        <v>11.07</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="8">
@@ -1299,28 +1401,28 @@
         <v>0.199</v>
       </c>
       <c r="D8" t="n">
-        <v>0.614</v>
+        <v>0.618</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0158</v>
+        <v>0.0153</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0007</v>
+        <v>0.0008</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0696</v>
+        <v>0.0655</v>
       </c>
       <c r="H8" t="n">
-        <v>1.22</v>
+        <v>1.25</v>
       </c>
       <c r="I8" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="J8" t="n">
-        <v>0.972</v>
+        <v>0.974</v>
       </c>
       <c r="K8" t="n">
-        <v>10.69</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="9">
@@ -1328,34 +1430,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.326</v>
+        <v>0.322</v>
       </c>
       <c r="C9" t="n">
-        <v>0.171</v>
+        <v>0.167</v>
       </c>
       <c r="D9" t="n">
-        <v>0.534</v>
+        <v>0.533</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0147</v>
+        <v>0.0133</v>
       </c>
       <c r="F9" t="n">
         <v>0.0007</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0622</v>
+        <v>0.0548</v>
       </c>
       <c r="H9" t="n">
-        <v>1.3</v>
+        <v>1.45</v>
       </c>
       <c r="I9" t="n">
-        <v>0.464</v>
+        <v>0.501</v>
       </c>
       <c r="J9" t="n">
-        <v>0.994</v>
+        <v>0.992</v>
       </c>
       <c r="K9" t="n">
-        <v>9.609999999999999</v>
+        <v>9.710000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -1363,34 +1465,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.318</v>
+        <v>0.328</v>
       </c>
       <c r="C10" t="n">
-        <v>0.162</v>
+        <v>0.171</v>
       </c>
       <c r="D10" t="n">
-        <v>0.523</v>
+        <v>0.535</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0145</v>
+        <v>0.0165</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.001</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0613</v>
+        <v>0.0654</v>
       </c>
       <c r="H10" t="n">
-        <v>1.33</v>
+        <v>1.17</v>
       </c>
       <c r="I10" t="n">
-        <v>0.471</v>
+        <v>0.424</v>
       </c>
       <c r="J10" t="n">
-        <v>0.991</v>
+        <v>0.992</v>
       </c>
       <c r="K10" t="n">
-        <v>9.390000000000001</v>
+        <v>9.359999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -1398,34 +1500,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.292</v>
+        <v>0.303</v>
       </c>
       <c r="C11" t="n">
-        <v>0.151</v>
+        <v>0.152</v>
       </c>
       <c r="D11" t="n">
-        <v>0.479</v>
+        <v>0.503</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0139</v>
+        <v>0.0143</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0005</v>
+        <v>0.0007</v>
       </c>
       <c r="G11" t="n">
-        <v>0.057</v>
+        <v>0.0595</v>
       </c>
       <c r="H11" t="n">
-        <v>1.38</v>
+        <v>1.35</v>
       </c>
       <c r="I11" t="n">
-        <v>0.485</v>
+        <v>0.475</v>
       </c>
       <c r="J11" t="n">
-        <v>0.998</v>
+        <v>0.981</v>
       </c>
       <c r="K11" t="n">
-        <v>8.77</v>
+        <v>8.890000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -1450,34 +1552,34 @@
         <v>2348</v>
       </c>
       <c r="B13" t="n">
-        <v>0.031</v>
+        <v>0.026</v>
       </c>
       <c r="C13" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="D13" t="n">
-        <v>0.142</v>
+        <v>0.129</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0317</v>
+        <v>0.035</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0009</v>
+        <v>0.0019</v>
       </c>
       <c r="G13" t="n">
-        <v>1.03</v>
+        <v>1.2343</v>
       </c>
       <c r="H13" t="n">
-        <v>0.61</v>
+        <v>0.55</v>
       </c>
       <c r="I13" t="n">
-        <v>0.193</v>
+        <v>0.162</v>
       </c>
       <c r="J13" t="n">
-        <v>0.281</v>
+        <v>0.254</v>
       </c>
       <c r="K13" t="n">
-        <v>0.19</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="14">
@@ -1485,34 +1587,34 @@
         <v>2349</v>
       </c>
       <c r="B14" t="n">
-        <v>0.03</v>
+        <v>0.028</v>
       </c>
       <c r="C14" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="D14" t="n">
-        <v>0.145</v>
+        <v>0.133</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0317</v>
+        <v>0.0352</v>
       </c>
       <c r="F14" t="n">
-        <v>0.001</v>
+        <v>0.0018</v>
       </c>
       <c r="G14" t="n">
-        <v>1.1113</v>
+        <v>1.3254</v>
       </c>
       <c r="H14" t="n">
-        <v>0.61</v>
+        <v>0.55</v>
       </c>
       <c r="I14" t="n">
-        <v>0.192</v>
+        <v>0.16</v>
       </c>
       <c r="J14" t="n">
-        <v>0.285</v>
+        <v>0.242</v>
       </c>
       <c r="K14" t="n">
-        <v>0.19</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="15">
@@ -1520,34 +1622,34 @@
         <v>2350</v>
       </c>
       <c r="B15" t="n">
-        <v>0.461</v>
+        <v>0.492</v>
       </c>
       <c r="C15" t="n">
-        <v>0.051</v>
+        <v>0.188</v>
       </c>
       <c r="D15" t="n">
-        <v>1.541</v>
+        <v>0.9379999999999999</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0439</v>
+        <v>0.0396</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0078</v>
+        <v>0.0071</v>
       </c>
       <c r="G15" t="n">
-        <v>0.9691</v>
+        <v>0.2426</v>
       </c>
       <c r="H15" t="n">
-        <v>0.44</v>
+        <v>0.49</v>
       </c>
       <c r="I15" t="n">
-        <v>0.102</v>
+        <v>0.128</v>
       </c>
       <c r="J15" t="n">
-        <v>0.022</v>
+        <v>0.014</v>
       </c>
       <c r="K15" t="n">
-        <v>0.19</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="16">
@@ -1555,34 +1657,34 @@
         <v>2351</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5</v>
+        <v>0.029</v>
       </c>
       <c r="C16" t="n">
-        <v>0.195</v>
+        <v>0.001</v>
       </c>
       <c r="D16" t="n">
-        <v>0.955</v>
+        <v>0.145</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0377</v>
+        <v>0.0358</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0053</v>
+        <v>0.0019</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2275</v>
+        <v>1.4293</v>
       </c>
       <c r="H16" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="I16" t="n">
-        <v>0.141</v>
+        <v>0.155</v>
       </c>
       <c r="J16" t="n">
-        <v>0.017</v>
+        <v>0.23</v>
       </c>
       <c r="K16" t="n">
-        <v>0.17</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="17">
@@ -1590,34 +1692,34 @@
         <v>2352</v>
       </c>
       <c r="B17" t="n">
-        <v>0.369</v>
+        <v>0.353</v>
       </c>
       <c r="C17" t="n">
-        <v>0.091</v>
+        <v>0.082</v>
       </c>
       <c r="D17" t="n">
-        <v>0.873</v>
+        <v>0.84</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0399</v>
+        <v>0.0389</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0056</v>
+        <v>0.0059</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3355</v>
+        <v>0.2982</v>
       </c>
       <c r="H17" t="n">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="I17" t="n">
-        <v>0.126</v>
+        <v>0.132</v>
       </c>
       <c r="J17" t="n">
-        <v>0.013</v>
+        <v>0.019</v>
       </c>
       <c r="K17" t="n">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="18">
@@ -1625,34 +1727,34 @@
         <v>2353</v>
       </c>
       <c r="B18" t="n">
-        <v>0.394</v>
+        <v>0.379</v>
       </c>
       <c r="C18" t="n">
-        <v>0.078</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>1.027</v>
+        <v>1.009</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0421</v>
+        <v>0.043</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0071</v>
+        <v>0.0083</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4646</v>
+        <v>0.4693</v>
       </c>
       <c r="H18" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="I18" t="n">
-        <v>0.112</v>
+        <v>0.107</v>
       </c>
       <c r="J18" t="n">
         <v>0.012</v>
       </c>
       <c r="K18" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="19">
@@ -1660,34 +1762,34 @@
         <v>2354</v>
       </c>
       <c r="B19" t="n">
-        <v>0.438</v>
+        <v>0.421</v>
       </c>
       <c r="C19" t="n">
-        <v>0.102</v>
+        <v>0.091</v>
       </c>
       <c r="D19" t="n">
-        <v>1.07</v>
+        <v>1.035</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0414</v>
+        <v>0.0434</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0069</v>
+        <v>0.0098</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4215</v>
+        <v>0.4399</v>
       </c>
       <c r="H19" t="n">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
       <c r="I19" t="n">
-        <v>0.116</v>
+        <v>0.105</v>
       </c>
       <c r="J19" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="K19" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="20">
@@ -1695,22 +1797,22 @@
         <v>2355</v>
       </c>
       <c r="B20" t="n">
-        <v>0.905</v>
+        <v>0.924</v>
       </c>
       <c r="C20" t="n">
-        <v>0.146</v>
+        <v>0.145</v>
       </c>
       <c r="D20" t="n">
-        <v>2.605</v>
+        <v>2.688</v>
       </c>
       <c r="E20" t="n">
         <v>0.0456</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0112</v>
+        <v>0.0118</v>
       </c>
       <c r="G20" t="n">
-        <v>1.2043</v>
+        <v>1.0989</v>
       </c>
       <c r="H20" t="n">
         <v>0.42</v>
@@ -1730,34 +1832,34 @@
         <v>2356</v>
       </c>
       <c r="B21" t="n">
-        <v>0.713</v>
+        <v>0.708</v>
       </c>
       <c r="C21" t="n">
-        <v>0.236</v>
+        <v>0.223</v>
       </c>
       <c r="D21" t="n">
-        <v>1.482</v>
+        <v>1.49</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0425</v>
+        <v>0.0411</v>
       </c>
       <c r="F21" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0073</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4207</v>
+        <v>0.3828</v>
       </c>
       <c r="H21" t="n">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="I21" t="n">
-        <v>0.11</v>
+        <v>0.118</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="K21" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="22">
@@ -1765,28 +1867,28 @@
         <v>2357</v>
       </c>
       <c r="B22" t="n">
-        <v>3.547</v>
+        <v>3.573</v>
       </c>
       <c r="C22" t="n">
-        <v>2.066</v>
+        <v>2.1</v>
       </c>
       <c r="D22" t="n">
-        <v>5.34</v>
+        <v>5.445</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0446</v>
+        <v>0.044</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0104</v>
+        <v>0.0094</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5867</v>
+        <v>0.5479000000000001</v>
       </c>
       <c r="H22" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="I22" t="n">
-        <v>0.098</v>
+        <v>0.102</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1802,31 +1904,31 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.059</v>
+        <v>0.057</v>
       </c>
       <c r="C23" t="n">
         <v>0.011</v>
       </c>
       <c r="D23" t="n">
-        <v>0.202</v>
+        <v>0.197</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0276</v>
+        <v>0.0271</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0009</v>
+        <v>0.0011</v>
       </c>
       <c r="G23" t="n">
-        <v>0.7879</v>
+        <v>0.5395</v>
       </c>
       <c r="H23" t="n">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="I23" t="n">
-        <v>0.255</v>
+        <v>0.26</v>
       </c>
       <c r="J23" t="n">
-        <v>0.443</v>
+        <v>0.453</v>
       </c>
       <c r="K23" t="n">
         <v>0.72</v>
@@ -1839,22 +1941,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.028</v>
+        <v>0.021</v>
       </c>
       <c r="C24" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="D24" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.077</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0118</v>
+        <v>0.011</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0004</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0517</v>
+        <v>0.0461</v>
       </c>
       <c r="H24" t="n">
         <v>0.42</v>
@@ -1876,34 +1978,34 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3.547</v>
+        <v>3.573</v>
       </c>
       <c r="C25" t="n">
-        <v>2.066</v>
+        <v>2.1</v>
       </c>
       <c r="D25" t="n">
-        <v>5.34</v>
+        <v>5.445</v>
       </c>
       <c r="E25" t="n">
         <v>0.0456</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0112</v>
+        <v>0.0118</v>
       </c>
       <c r="G25" t="n">
-        <v>14.8072</v>
+        <v>8.953900000000001</v>
       </c>
       <c r="H25" t="n">
-        <v>1.62</v>
+        <v>1.76</v>
       </c>
       <c r="I25" t="n">
-        <v>0.54</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>21.78</v>
+        <v>21.69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>